<commit_message>
Add a performance table
</commit_message>
<xml_diff>
--- a/tabela-wydajnosci-i-cele.xlsx
+++ b/tabela-wydajnosci-i-cele.xlsx
@@ -1,19 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleksandrakaminska/Desktop/frontend-optimisation-starter-kit/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A24501C-62C5-674B-BC55-77345590D2D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="17380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Podsumowanie eksportu" sheetId="1" r:id="rId4"/>
-    <sheet name="Na czym nam zależy_ - Obecny i " sheetId="2" r:id="rId5"/>
-    <sheet name="Tabela wydajności" sheetId="3" r:id="rId6"/>
+    <sheet name="Podsumowanie eksportu" sheetId="1" r:id="rId1"/>
+    <sheet name="Na czym nam zależy_ - Obecny i " sheetId="2" r:id="rId2"/>
+    <sheet name="Tabela wydajności" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Ten dokument został wyeksportowany z aplikacji Numbers. Każda z tabel została skonwertowana do arkusza aplikacji Excel. Pozostałe obiekty na każdym z arkuszy Numbers zostały umieszczone na osobnych arkuszach. Pamiętaj, że działanie formuł w aplikacji Excel może być inne.</t>
   </si>
@@ -96,29 +116,32 @@
     <t>Lighthouse</t>
   </si>
   <si>
-    <t>Typ strony 1</t>
-  </si>
-  <si>
-    <t>Typ strony 2</t>
-  </si>
-  <si>
-    <t>Typ strony 3</t>
-  </si>
-  <si>
-    <t>Typ strony 4</t>
-  </si>
-  <si>
     <t>Zmienność</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Homepage</t>
+  </si>
+  <si>
+    <t>cta-ad</t>
+  </si>
+  <si>
+    <t>news listing</t>
+  </si>
+  <si>
+    <t>news single</t>
+  </si>
+  <si>
+    <t>partners</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -135,13 +158,13 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="12"/>
       <color indexed="11"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -152,18 +175,13 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,42 +224,8 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <gradientFill type="linear" degree="90">
-        <stop position="0">
-          <color rgb="fffe968c"/>
-        </stop>
-        <stop position="1">
-          <color rgb="ffed220b"/>
-        </stop>
-      </gradientFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="19"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="20"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="21"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="22"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="15">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -397,26 +381,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="17"/>
-      </left>
-      <right style="thin">
-        <color indexed="17"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="17"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="17"/>
       </left>
@@ -433,112 +397,76 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="26">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -548,36 +476,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="015e88b1"/>
-      <rgbColor rgb="01eef3f4"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ffd5d5d5"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="fff9f9f9"/>
-      <rgbColor rgb="fffe634d"/>
-      <rgbColor rgb="ff88f94e"/>
-      <rgbColor rgb="ffff968c"/>
-      <rgbColor rgb="ffed220b"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="015E88B1"/>
+      <rgbColor rgb="01EEF3F4"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FFD5D5D5"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFF9F9F9"/>
+      <rgbColor rgb="FFFE634D"/>
+      <rgbColor rgb="FF88F94E"/>
+      <rgbColor rgb="FFFF968C"/>
+      <rgbColor rgb="FFED220B"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -776,7 +753,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -795,7 +772,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -825,7 +802,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -851,7 +828,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -877,7 +854,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -903,7 +880,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -929,7 +906,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -955,7 +932,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -981,7 +958,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1007,7 +984,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1033,7 +1010,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1046,9 +1023,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1065,7 +1048,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1084,7 +1067,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1110,7 +1093,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1136,7 +1119,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1162,7 +1145,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1188,7 +1171,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1214,7 +1197,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1240,7 +1223,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1266,7 +1249,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1292,7 +1275,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1318,7 +1301,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1331,9 +1314,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1347,7 +1336,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1366,7 +1355,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1396,7 +1385,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1422,7 +1411,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1448,7 +1437,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1474,7 +1463,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1500,7 +1489,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1526,7 +1515,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1552,7 +1541,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1578,7 +1567,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1604,7 +1593,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1617,74 +1606,82 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="4" width="33.6016" customWidth="1"/>
+    <col min="2" max="4" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="50" customHeight="1">
-      <c r="B3" t="s" s="1">
+    <row r="3" spans="2:4" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
-    </row>
-    <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+    </row>
+    <row r="7" spans="2:4" ht="38" x14ac:dyDescent="0.15">
+      <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9">
-      <c r="B9" t="s" s="3">
+    <row r="9" spans="2:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="2:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
+      <c r="D10" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" t="s" s="3">
+    <row r="11" spans="2:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="4"/>
-      <c r="C12" t="s" s="4">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="2:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D12" t="s" s="5">
+      <c r="D12" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1693,130 +1690,135 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D10" location="'Na czym nam zależy_ - Obecny i '!R2C1" tooltip="" display="Na czym nam zależy_ - Obecny i "/>
-    <hyperlink ref="D12" location="'Tabela wydajności'!R1C1" tooltip="" display="Tabela wydajności"/>
+    <hyperlink ref="D10" location="'Na czym nam zależy_ - Obecny i '!R2C1" display="Na czym nam zależy_ - Obecny i " xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D12" location="'Tabela wydajności'!R1C1" display="Tabela wydajności" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:D11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="55.9219" style="6" customWidth="1"/>
-    <col min="2" max="2" width="31.4062" style="6" customWidth="1"/>
-    <col min="3" max="3" width="32.2031" style="6" customWidth="1"/>
-    <col min="4" max="4" width="29.8438" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="16.3516" style="6" customWidth="1"/>
+    <col min="1" max="1" width="56" style="5" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="32.1640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="29.83203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="16.33203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="7">
+    <row r="1" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-    </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="8">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+    </row>
+    <row r="2" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s" s="8">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s" s="8">
+      <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s" s="8">
+      <c r="D2" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="9">
+    <row r="3" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="8">
         <v>0.92</v>
       </c>
-      <c r="C3" t="s" s="11">
+      <c r="C3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="10">
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="13">
+    <row r="4" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s" s="14">
+      <c r="B4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s" s="15">
+      <c r="C4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s" s="15">
+      <c r="D4" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="16"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
+    <row r="5" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1824,248 +1826,268 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19.3984" style="19" customWidth="1"/>
-    <col min="2" max="2" width="17.9141" style="19" customWidth="1"/>
-    <col min="3" max="3" width="15.3516" style="19" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="19" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="19" customWidth="1"/>
-    <col min="6" max="6" width="15.3516" style="19" customWidth="1"/>
-    <col min="7" max="8" width="16.3516" style="19" customWidth="1"/>
-    <col min="9" max="9" width="14.5" style="19" customWidth="1"/>
-    <col min="10" max="16384" width="14.5" style="19" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="17" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="17" customWidth="1"/>
+    <col min="7" max="8" width="16.33203125" style="17" customWidth="1"/>
+    <col min="9" max="10" width="14.5" style="17" customWidth="1"/>
+    <col min="11" max="16384" width="14.5" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" s="20"/>
-      <c r="B1" t="s" s="21">
+    <row r="1" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="18"/>
+      <c r="B1" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s" s="21">
+      <c r="C1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s" s="21">
+      <c r="D1" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s" s="21">
+      <c r="E1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s" s="21">
+      <c r="F1" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s" s="21">
+      <c r="G1" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s" s="21">
+      <c r="H1" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s" s="22">
+      <c r="I1" s="20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="23">
+    <row r="2" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="22">
+        <v>4.7E-2</v>
+      </c>
+      <c r="C2" s="22">
+        <v>0.7</v>
+      </c>
+      <c r="D2" s="22">
+        <v>0.7</v>
+      </c>
+      <c r="E2" s="22">
+        <v>2.9</v>
+      </c>
+      <c r="F2" s="22">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G2" s="22">
+        <v>0.09</v>
+      </c>
+      <c r="H2" s="22">
+        <v>0.7</v>
+      </c>
+      <c r="I2" s="22">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="22">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C3" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="F3" s="22">
+        <v>0.9</v>
+      </c>
+      <c r="G3" s="22">
+        <v>0.01</v>
+      </c>
+      <c r="H3" s="22">
+        <v>0.7</v>
+      </c>
+      <c r="I3" s="22">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="22">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C4" s="22">
+        <v>0.104</v>
+      </c>
+      <c r="D4" s="22">
+        <v>0.105</v>
+      </c>
+      <c r="E4" s="22">
+        <v>0.105</v>
+      </c>
+      <c r="F4" s="22">
+        <v>0.105</v>
+      </c>
+      <c r="G4" s="22">
+        <v>0</v>
+      </c>
+      <c r="H4" s="22">
+        <v>0</v>
+      </c>
+      <c r="I4" s="22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="22">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="C5" s="22">
+        <v>0.6</v>
+      </c>
+      <c r="D5" s="22">
+        <v>0.6</v>
+      </c>
+      <c r="E5" s="22">
+        <v>1.8</v>
+      </c>
+      <c r="F5" s="22">
+        <v>1.9</v>
+      </c>
+      <c r="G5" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="H5" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="I5" s="22">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="22">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="C6" s="22">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="D6" s="22">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="E6" s="22">
+        <v>1.2</v>
+      </c>
+      <c r="F6" s="22">
+        <v>1.4</v>
+      </c>
+      <c r="G6" s="22">
+        <v>0.24</v>
+      </c>
+      <c r="H6" s="22">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="I6" s="22">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="22">
+        <v>0.04</v>
+      </c>
+      <c r="C7" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="22">
+        <v>2.6</v>
+      </c>
+      <c r="F7" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="G7" s="22">
+        <v>0.01</v>
+      </c>
+      <c r="H7" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="I7" s="22">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="24">
-        <v>1.164</v>
-      </c>
-      <c r="C2" s="24">
-        <v>1.8</v>
-      </c>
-      <c r="D2" s="24">
-        <v>3.139</v>
-      </c>
-      <c r="E2" s="24">
-        <v>4.791</v>
-      </c>
-      <c r="F2" s="24">
-        <v>1.073</v>
-      </c>
-      <c r="G2" s="24">
-        <v>0.032</v>
-      </c>
-      <c r="H2" s="24">
-        <v>0.106</v>
-      </c>
-      <c r="I2" s="25">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="23">
-        <v>28</v>
-      </c>
-      <c r="B3" s="24">
-        <v>1.78</v>
-      </c>
-      <c r="C3" s="26">
-        <v>6.281</v>
-      </c>
-      <c r="D3" s="24">
-        <v>3.901</v>
-      </c>
-      <c r="E3" s="26">
-        <v>6.781</v>
-      </c>
-      <c r="F3" s="26">
-        <v>18.98</v>
-      </c>
-      <c r="G3" s="27">
-        <v>1.036</v>
-      </c>
-      <c r="H3" s="24">
-        <v>0.128</v>
-      </c>
-      <c r="I3" s="25">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" t="s" s="23">
-        <v>29</v>
-      </c>
-      <c r="B4" s="24">
-        <v>1.261</v>
-      </c>
-      <c r="C4" s="24">
-        <v>1.9</v>
-      </c>
-      <c r="D4" s="24">
-        <v>3.91</v>
-      </c>
-      <c r="E4" s="24">
-        <v>4.776</v>
-      </c>
-      <c r="F4" s="24">
-        <v>3.215</v>
-      </c>
-      <c r="G4" s="24">
-        <v>0.005</v>
-      </c>
-      <c r="H4" s="24">
-        <v>0.663</v>
-      </c>
-      <c r="I4" s="25">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="23">
-        <v>30</v>
-      </c>
-      <c r="B5" s="24">
-        <v>1.787</v>
-      </c>
-      <c r="C5" s="24">
-        <v>3.148</v>
-      </c>
-      <c r="D5" s="24">
-        <v>3.21</v>
-      </c>
-      <c r="E5" s="24">
-        <v>5.021</v>
-      </c>
-      <c r="F5" s="24">
-        <v>2.648</v>
-      </c>
-      <c r="G5" s="24">
-        <v>0.876</v>
-      </c>
-      <c r="H5" s="24">
-        <v>0.125</v>
-      </c>
-      <c r="I5" s="25">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" t="s" s="23">
-        <v>31</v>
-      </c>
-      <c r="B6" s="28">
-        <f>STDEV(B2:B5)</f>
-        <v>0.332049193142623</v>
-      </c>
-      <c r="C6" s="27">
-        <f>STDEV(C2:C5)</f>
-        <v>2.09110853775376</v>
-      </c>
-      <c r="D6" s="24">
-        <f>STDEV(D2:D5)</f>
-        <v>0.423053188145415</v>
-      </c>
-      <c r="E6" s="29">
-        <f>STDEV(E2:E5)</f>
-        <v>0.96569814987224</v>
-      </c>
-      <c r="F6" s="30">
-        <f>STDEV(F2:F5)</f>
-        <v>8.38311982498163</v>
-      </c>
-      <c r="G6" s="24">
-        <f>STDEV(G2:G5)</f>
-        <v>0.545304425680433</v>
-      </c>
-      <c r="H6" s="28">
-        <f>STDEV(H2:H5)</f>
-        <v>0.271841252694779</v>
-      </c>
-      <c r="I6" s="31"/>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="33"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-    </row>
+      <c r="B8" s="22">
+        <f>STDEV(B2:B7)</f>
+        <v>4.0353438515199666E-2</v>
+      </c>
+      <c r="C8" s="22">
+        <f>STDEV(C2:C7)</f>
+        <v>0.20379466790538631</v>
+      </c>
+      <c r="D8" s="22">
+        <f>STDEV(D2:D7)</f>
+        <v>0.20343426456720604</v>
+      </c>
+      <c r="E8" s="22">
+        <f>STDEV(E2:E7)</f>
+        <v>1.0731903372654823</v>
+      </c>
+      <c r="F8" s="22">
+        <f>STDEV(F2:F7)</f>
+        <v>0.79774943852482039</v>
+      </c>
+      <c r="G8" s="22">
+        <f>STDEV(G2:G7)</f>
+        <v>0.1053407170407847</v>
+      </c>
+      <c r="H8" s="22">
+        <f>STDEV(H2:H7)</f>
+        <v>0.49079544279329512</v>
+      </c>
+      <c r="I8" s="22"/>
+    </row>
+    <row r="9" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup scale="72" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>